<commit_message>
updated links for website project section
</commit_message>
<xml_diff>
--- a/bugs_and_features.xlsx
+++ b/bugs_and_features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smit/Documents/smit-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E95B921-3F6C-F945-B797-BCBB701891DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9CB0A3-4B72-7B49-8673-986A78FD8D86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19820" xr2:uid="{5C0D04F8-EFD7-D94A-AEB9-27970217DD0D}"/>
   </bookViews>
@@ -549,7 +549,7 @@
   <dimension ref="B2:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,7 +607,7 @@
       </c>
       <c r="F4" s="5">
         <f ca="1">TODAY()</f>
-        <v>44321</v>
+        <v>44322</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
@@ -700,38 +700,40 @@
       </c>
       <c r="F10" s="5">
         <f ca="1">TODAY()</f>
-        <v>44321</v>
+        <v>44322</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="6">
-        <v>3</v>
-      </c>
-      <c r="E11" s="7">
-        <v>44320</v>
-      </c>
-      <c r="F11" s="6"/>
+      <c r="D11" s="4">
+        <v>3</v>
+      </c>
+      <c r="E11" s="5">
+        <v>44320</v>
+      </c>
+      <c r="F11" s="5">
+        <v>44322</v>
+      </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="2">
-        <v>3</v>
-      </c>
-      <c r="E12" s="3">
-        <v>44320</v>
-      </c>
-      <c r="F12" s="2"/>
+      <c r="D12" s="6">
+        <v>3</v>
+      </c>
+      <c r="E12" s="7">
+        <v>44320</v>
+      </c>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
@@ -897,7 +899,7 @@
       </c>
       <c r="E23" s="3">
         <f ca="1">TODAY()</f>
-        <v>44321</v>
+        <v>44322</v>
       </c>
       <c r="F23" s="2"/>
     </row>

</xml_diff>

<commit_message>
Fixed button hover bug for safari
</commit_message>
<xml_diff>
--- a/bugs_and_features.xlsx
+++ b/bugs_and_features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smit/Documents/smit-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9CB0A3-4B72-7B49-8673-986A78FD8D86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8E22B5-233F-EF44-86D2-578BDAA756BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19820" xr2:uid="{5C0D04F8-EFD7-D94A-AEB9-27970217DD0D}"/>
   </bookViews>
@@ -549,7 +549,7 @@
   <dimension ref="B2:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,8 +606,7 @@
         <v>44320</v>
       </c>
       <c r="F4" s="5">
-        <f ca="1">TODAY()</f>
-        <v>44322</v>
+        <v>44321</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
@@ -699,8 +698,7 @@
         <v>44320</v>
       </c>
       <c r="F10" s="5">
-        <f ca="1">TODAY()</f>
-        <v>44322</v>
+        <v>44321</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
@@ -721,19 +719,21 @@
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="6">
-        <v>3</v>
-      </c>
-      <c r="E12" s="7">
-        <v>44320</v>
-      </c>
-      <c r="F12" s="6"/>
+      <c r="D12" s="4">
+        <v>3</v>
+      </c>
+      <c r="E12" s="5">
+        <v>44320</v>
+      </c>
+      <c r="F12" s="5">
+        <v>44322</v>
+      </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
@@ -826,19 +826,19 @@
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="2">
-        <v>3</v>
-      </c>
-      <c r="E19" s="3">
-        <v>44320</v>
-      </c>
-      <c r="F19" s="2"/>
+      <c r="D19" s="6">
+        <v>3</v>
+      </c>
+      <c r="E19" s="7">
+        <v>44320</v>
+      </c>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">

</xml_diff>

<commit_message>
Fixed Safari font size bug. Refactored font sizes. Changed coming soon page design.
</commit_message>
<xml_diff>
--- a/bugs_and_features.xlsx
+++ b/bugs_and_features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smit/Documents/smit-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8E22B5-233F-EF44-86D2-578BDAA756BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E3D175-0B07-7046-94DE-7D6593750126}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19820" xr2:uid="{5C0D04F8-EFD7-D94A-AEB9-27970217DD0D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>Task</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Small font size won't resize (Safari)</t>
   </si>
   <si>
-    <t>CN Tower SVG vertical height bug</t>
-  </si>
-  <si>
     <t>Feature</t>
   </si>
   <si>
@@ -124,6 +121,12 @@
   </si>
   <si>
     <t>Currently working on.</t>
+  </si>
+  <si>
+    <t>Safari white glow from ham button</t>
+  </si>
+  <si>
+    <t>Blur effect firefox</t>
   </si>
 </sst>
 </file>
@@ -214,7 +217,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -228,8 +231,11 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -546,16 +552,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C501BF-4B64-574E-831C-5EDD301DE290}">
-  <dimension ref="B2:F29"/>
+  <dimension ref="B2:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="38.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="8" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" customWidth="1"/>
   </cols>
@@ -570,7 +576,7 @@
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -582,7 +588,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2">
         <v>3</v>
@@ -597,7 +603,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="4">
         <v>4</v>
@@ -614,7 +620,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2">
         <v>2</v>
@@ -629,7 +635,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2">
         <v>3</v>
@@ -644,7 +650,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="2">
         <v>4</v>
@@ -659,7 +665,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2">
         <v>3</v>
@@ -674,7 +680,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2">
         <v>2</v>
@@ -689,7 +695,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="4">
         <v>2</v>
@@ -706,7 +712,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="4">
         <v>3</v>
@@ -723,7 +729,7 @@
         <v>14</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="4">
         <v>3</v>
@@ -740,7 +746,7 @@
         <v>15</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2">
         <v>2</v>
@@ -755,7 +761,7 @@
         <v>16</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="2">
         <v>2</v>
@@ -767,10 +773,10 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" s="2">
         <v>3</v>
@@ -781,26 +787,26 @@
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="2">
+      <c r="C16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="6">
         <v>1</v>
       </c>
-      <c r="E16" s="3">
-        <v>44320</v>
-      </c>
-      <c r="F16" s="2"/>
+      <c r="E16" s="7">
+        <v>44320</v>
+      </c>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="2">
         <v>1</v>
@@ -815,108 +821,125 @@
         <v>19</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="2">
+        <v>3</v>
+      </c>
+      <c r="E18" s="3">
+        <v>44320</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="2">
-        <v>3</v>
-      </c>
-      <c r="E18" s="3">
-        <v>44320</v>
-      </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="2">
+        <v>3</v>
+      </c>
+      <c r="E19" s="3">
+        <v>44320</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="4">
+        <v>3</v>
+      </c>
+      <c r="E20" s="5">
+        <v>44320</v>
+      </c>
+      <c r="F20" s="5">
+        <v>44322</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="6">
-        <v>3</v>
-      </c>
-      <c r="E19" s="7">
-        <v>44320</v>
-      </c>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="2">
-        <v>3</v>
-      </c>
-      <c r="E20" s="3">
-        <v>44320</v>
-      </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="2">
-        <v>3</v>
-      </c>
-      <c r="E21" s="3">
-        <v>44320</v>
-      </c>
-      <c r="F21" s="2"/>
+      <c r="C21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="4">
+        <v>4</v>
+      </c>
+      <c r="E21" s="5">
+        <v>44320</v>
+      </c>
+      <c r="F21" s="5">
+        <v>44320</v>
+      </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="4">
-        <v>4</v>
-      </c>
-      <c r="E22" s="5">
-        <v>44320</v>
-      </c>
-      <c r="F22" s="5">
-        <v>44320</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="2">
-        <v>3</v>
-      </c>
-      <c r="E23" s="3">
+      <c r="C22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="2">
+        <v>3</v>
+      </c>
+      <c r="E22" s="3">
         <f ca="1">TODAY()</f>
         <v>44322</v>
       </c>
-      <c r="F23" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="6">
+        <v>2</v>
+      </c>
+      <c r="E23" s="7">
+        <v>44322</v>
+      </c>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="2">
+        <v>2</v>
+      </c>
+      <c r="E24" s="3">
+        <v>44322</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E26" s="13"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E27" s="11"/>
+      <c r="B27" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="11"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="12"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B29" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="8"/>
+      <c r="D28" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed some warnings and errors displayed in console.
</commit_message>
<xml_diff>
--- a/bugs_and_features.xlsx
+++ b/bugs_and_features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smit/Documents/smit-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E3D175-0B07-7046-94DE-7D6593750126}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546CEAFA-5488-5142-9AD6-C0D27F8E7DF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19820" xr2:uid="{5C0D04F8-EFD7-D94A-AEB9-27970217DD0D}"/>
   </bookViews>
@@ -123,10 +123,10 @@
     <t>Currently working on.</t>
   </si>
   <si>
-    <t>Safari white glow from ham button</t>
-  </si>
-  <si>
     <t>Blur effect firefox</t>
+  </si>
+  <si>
+    <t>White glow from ham button</t>
   </si>
 </sst>
 </file>
@@ -555,7 +555,7 @@
   <dimension ref="B2:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,19 +616,19 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="6">
         <v>2</v>
       </c>
-      <c r="E5" s="3">
-        <v>44320</v>
-      </c>
-      <c r="F5" s="2"/>
+      <c r="E5" s="7">
+        <v>44320</v>
+      </c>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -881,39 +881,40 @@
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="2">
-        <v>3</v>
-      </c>
-      <c r="E22" s="3">
-        <f ca="1">TODAY()</f>
+      <c r="D22" s="6">
+        <v>3</v>
+      </c>
+      <c r="E22" s="7">
+        <v>44320</v>
+      </c>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2</v>
+      </c>
+      <c r="E23" s="5">
         <v>44322</v>
       </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="6">
-        <v>2</v>
-      </c>
-      <c r="E23" s="7">
+      <c r="F23" s="5">
         <v>44322</v>
       </c>
-      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Fixed mobile layout for experience section. Added more information in timeline section. Added pointer cursor for hover elements on experience page.
</commit_message>
<xml_diff>
--- a/bugs_and_features.xlsx
+++ b/bugs_and_features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smit/Documents/smit-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546CEAFA-5488-5142-9AD6-C0D27F8E7DF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231068F9-B3D2-F54D-844E-EBE23EC3E58B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19820" xr2:uid="{5C0D04F8-EFD7-D94A-AEB9-27970217DD0D}"/>
   </bookViews>
@@ -217,7 +217,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -236,6 +236,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -555,7 +557,7 @@
   <dimension ref="B2:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,64 +618,68 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="6">
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2">
         <v>2</v>
       </c>
-      <c r="E5" s="7">
-        <v>44320</v>
-      </c>
-      <c r="F5" s="6"/>
+      <c r="E5" s="3">
+        <v>44320</v>
+      </c>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="2">
-        <v>3</v>
-      </c>
-      <c r="E6" s="3">
-        <v>44320</v>
-      </c>
-      <c r="F6" s="2"/>
+      <c r="C6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5">
+        <v>44320</v>
+      </c>
+      <c r="F6" s="5">
+        <v>44325</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4">
         <v>4</v>
       </c>
-      <c r="E7" s="3">
-        <v>44320</v>
-      </c>
-      <c r="F7" s="2"/>
+      <c r="E7" s="5">
+        <v>44320</v>
+      </c>
+      <c r="F7" s="5">
+        <v>44325</v>
+      </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="2">
-        <v>3</v>
-      </c>
-      <c r="E8" s="3">
-        <v>44320</v>
-      </c>
-      <c r="F8" s="2"/>
+      <c r="D8" s="14">
+        <v>3</v>
+      </c>
+      <c r="E8" s="15">
+        <v>44320</v>
+      </c>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
@@ -772,34 +778,36 @@
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="2">
-        <v>3</v>
-      </c>
-      <c r="E15" s="3">
-        <v>44320</v>
-      </c>
-      <c r="F15" s="2"/>
+      <c r="C15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="4">
+        <v>3</v>
+      </c>
+      <c r="E15" s="5">
+        <v>44320</v>
+      </c>
+      <c r="F15" s="5">
+        <v>44325</v>
+      </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="6">
+      <c r="C16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="2">
         <v>1</v>
       </c>
-      <c r="E16" s="7">
-        <v>44320</v>
-      </c>
-      <c r="F16" s="6"/>
+      <c r="E16" s="3">
+        <v>44320</v>
+      </c>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
@@ -832,19 +840,19 @@
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="2">
-        <v>3</v>
-      </c>
-      <c r="E19" s="3">
-        <v>44320</v>
-      </c>
-      <c r="F19" s="2"/>
+      <c r="D19" s="6">
+        <v>3</v>
+      </c>
+      <c r="E19" s="7">
+        <v>44320</v>
+      </c>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">

</xml_diff>

<commit_message>
Changes to improve SEO (meta tags). Added favicon images for different devices.
</commit_message>
<xml_diff>
--- a/bugs_and_features.xlsx
+++ b/bugs_and_features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smit/Documents/smit-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231068F9-B3D2-F54D-844E-EBE23EC3E58B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E12C477-C02F-EE41-A150-5C308ED9BF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19820" xr2:uid="{5C0D04F8-EFD7-D94A-AEB9-27970217DD0D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{5C0D04F8-EFD7-D94A-AEB9-27970217DD0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t>Task</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>White glow from ham button</t>
+  </si>
+  <si>
+    <t>Improve SEO</t>
   </si>
 </sst>
 </file>
@@ -557,7 +560,7 @@
   <dimension ref="B2:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -935,6 +938,23 @@
       </c>
       <c r="F24" s="2"/>
     </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="4">
+        <v>3</v>
+      </c>
+      <c r="E25" s="5">
+        <v>44330</v>
+      </c>
+      <c r="F25" s="5">
+        <v>44330</v>
+      </c>
+    </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E26" s="13"/>
     </row>

</xml_diff>

<commit_message>
Updated links for new domain.
</commit_message>
<xml_diff>
--- a/bugs_and_features.xlsx
+++ b/bugs_and_features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smit/Documents/smit-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E12C477-C02F-EE41-A150-5C308ED9BF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADA5F92-71DA-8242-B14E-1C9E824FDBE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{5C0D04F8-EFD7-D94A-AEB9-27970217DD0D}"/>
   </bookViews>
@@ -111,9 +111,6 @@
     <t>Screen Clipping</t>
   </si>
   <si>
-    <t>Error Warnings</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hover and hover cursor for timeline graph. </t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>Improve SEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error Warnings (Accessibility) </t>
   </si>
 </sst>
 </file>
@@ -560,7 +560,7 @@
   <dimension ref="B2:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -782,7 +782,7 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>22</v>
@@ -813,19 +813,21 @@
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="2">
+      <c r="C17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="4">
         <v>1</v>
       </c>
-      <c r="E17" s="3">
-        <v>44320</v>
-      </c>
-      <c r="F17" s="2"/>
+      <c r="E17" s="5">
+        <v>44320</v>
+      </c>
+      <c r="F17" s="5">
+        <v>44331</v>
+      </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
@@ -893,7 +895,7 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>23</v>
@@ -908,7 +910,7 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>23</v>
@@ -925,7 +927,7 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>23</v>
@@ -940,7 +942,7 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>22</v>
@@ -960,13 +962,13 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27" s="11"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="8"/>
     </row>

</xml_diff>